<commit_message>
modwt analysis and trikinetics free run cohort list update
</commit_message>
<xml_diff>
--- a/Data/2017-10-12_trik_cohort_list_free_run.xlsx
+++ b/Data/2017-10-12_trik_cohort_list_free_run.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="22620" yWindow="9560" windowWidth="26360" windowHeight="16380" tabRatio="500"/>
+    <workbookView xWindow="23220" yWindow="11020" windowWidth="26360" windowHeight="16380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="143">
   <si>
     <t>2017-09-26</t>
   </si>
@@ -276,6 +276,186 @@
   </si>
   <si>
     <t>2017-11-08</t>
+  </si>
+  <si>
+    <t>2017-11-09</t>
+  </si>
+  <si>
+    <t>2017-11-10</t>
+  </si>
+  <si>
+    <t>2017-11-11</t>
+  </si>
+  <si>
+    <t>2017-11-12</t>
+  </si>
+  <si>
+    <t>2017-11-13</t>
+  </si>
+  <si>
+    <t>2017-11-14</t>
+  </si>
+  <si>
+    <t>2017-11-15</t>
+  </si>
+  <si>
+    <t>2017-11-16</t>
+  </si>
+  <si>
+    <t>2017-11-17</t>
+  </si>
+  <si>
+    <t>2017-11-18</t>
+  </si>
+  <si>
+    <t>2017-11-19</t>
+  </si>
+  <si>
+    <t>2017-11-20</t>
+  </si>
+  <si>
+    <t>2017-11-21</t>
+  </si>
+  <si>
+    <t>2017-11-22</t>
+  </si>
+  <si>
+    <t>2017-11-23</t>
+  </si>
+  <si>
+    <t>2017-11-24</t>
+  </si>
+  <si>
+    <t>2017-11-25</t>
+  </si>
+  <si>
+    <t>2017-11-26</t>
+  </si>
+  <si>
+    <t>2017-11-27</t>
+  </si>
+  <si>
+    <t>2017-11-28</t>
+  </si>
+  <si>
+    <t>2017-11-29</t>
+  </si>
+  <si>
+    <t>2017-11-30</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>39</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>45</t>
+  </si>
+  <si>
+    <t>46</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>53</t>
+  </si>
+  <si>
+    <t>54</t>
+  </si>
+  <si>
+    <t>55</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>57</t>
+  </si>
+  <si>
+    <t>58</t>
+  </si>
+  <si>
+    <t>59</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>61</t>
+  </si>
+  <si>
+    <t>62</t>
+  </si>
+  <si>
+    <t>63</t>
+  </si>
+  <si>
+    <t>64</t>
+  </si>
+  <si>
+    <t>65</t>
+  </si>
+  <si>
+    <t>66</t>
+  </si>
+  <si>
+    <t>2017-12-01</t>
+  </si>
+  <si>
+    <t>2017-12-02</t>
+  </si>
+  <si>
+    <t>2017-12-03</t>
+  </si>
+  <si>
+    <t>2017-12-04</t>
+  </si>
+  <si>
+    <t>2017-12-05</t>
+  </si>
+  <si>
+    <t>2017-12-06</t>
+  </si>
+  <si>
+    <t>2017-12-07</t>
+  </si>
+  <si>
+    <t>2017-12-08</t>
   </si>
 </sst>
 </file>
@@ -617,10 +797,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C67"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="M69" sqref="M69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1037,6 +1217,336 @@
         <v>82</v>
       </c>
     </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updating entrainment to free run datasheets
</commit_message>
<xml_diff>
--- a/Data/2017-10-12_trik_cohort_list_free_run.xlsx
+++ b/Data/2017-10-12_trik_cohort_list_free_run.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="23220" yWindow="11020" windowWidth="26360" windowHeight="16380" tabRatio="500"/>
+    <workbookView xWindow="23220" yWindow="11020" windowWidth="26360" windowHeight="16380" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Free Run" sheetId="1" r:id="rId1"/>
+    <sheet name="Simulated Overwintering" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="432">
   <si>
     <t>2017-09-26</t>
   </si>
@@ -594,12 +595,741 @@
   </si>
   <si>
     <t>89</t>
+  </si>
+  <si>
+    <t>2018-02-12</t>
+  </si>
+  <si>
+    <t>2018-02-20</t>
+  </si>
+  <si>
+    <t>2018-02-13</t>
+  </si>
+  <si>
+    <t>2018-02-21</t>
+  </si>
+  <si>
+    <t>2018-02-22</t>
+  </si>
+  <si>
+    <t>2018-02-23</t>
+  </si>
+  <si>
+    <t>2018-02-24</t>
+  </si>
+  <si>
+    <t>2018-02-25</t>
+  </si>
+  <si>
+    <t>2018-02-26</t>
+  </si>
+  <si>
+    <t>2018-02-27</t>
+  </si>
+  <si>
+    <t>2018-02-28</t>
+  </si>
+  <si>
+    <t>2018-02-14</t>
+  </si>
+  <si>
+    <t>2018-02-15</t>
+  </si>
+  <si>
+    <t>2018-02-16</t>
+  </si>
+  <si>
+    <t>2018-02-17</t>
+  </si>
+  <si>
+    <t>2018-02-18</t>
+  </si>
+  <si>
+    <t>2018-02-19</t>
+  </si>
+  <si>
+    <t>2018-03-01</t>
+  </si>
+  <si>
+    <t>2018-03-02</t>
+  </si>
+  <si>
+    <t>2018-03-03</t>
+  </si>
+  <si>
+    <t>2018-03-04</t>
+  </si>
+  <si>
+    <t>2018-03-05</t>
+  </si>
+  <si>
+    <t>2018-03-06</t>
+  </si>
+  <si>
+    <t>2018-03-07</t>
+  </si>
+  <si>
+    <t>2018-03-08</t>
+  </si>
+  <si>
+    <t>2018-03-09</t>
+  </si>
+  <si>
+    <t>2018-03-10</t>
+  </si>
+  <si>
+    <t>2018-03-11</t>
+  </si>
+  <si>
+    <t>2018-03-12</t>
+  </si>
+  <si>
+    <t>2018-03-13</t>
+  </si>
+  <si>
+    <t>2018-03-14</t>
+  </si>
+  <si>
+    <t>2018-03-15</t>
+  </si>
+  <si>
+    <t>2018-03-16</t>
+  </si>
+  <si>
+    <t>2018-03-17</t>
+  </si>
+  <si>
+    <t>2018-03-18</t>
+  </si>
+  <si>
+    <t>2018-03-19</t>
+  </si>
+  <si>
+    <t>2018-03-20</t>
+  </si>
+  <si>
+    <t>2018-03-21</t>
+  </si>
+  <si>
+    <t>2018-03-22</t>
+  </si>
+  <si>
+    <t>2018-03-23</t>
+  </si>
+  <si>
+    <t>2018-03-24</t>
+  </si>
+  <si>
+    <t>2018-03-25</t>
+  </si>
+  <si>
+    <t>2018-03-26</t>
+  </si>
+  <si>
+    <t>2018-03-27</t>
+  </si>
+  <si>
+    <t>2018-03-28</t>
+  </si>
+  <si>
+    <t>2018-03-29</t>
+  </si>
+  <si>
+    <t>2018-03-30</t>
+  </si>
+  <si>
+    <t>2018-03-31</t>
+  </si>
+  <si>
+    <t>2018-04-01</t>
+  </si>
+  <si>
+    <t>2018-04-02</t>
+  </si>
+  <si>
+    <t>2018-04-03</t>
+  </si>
+  <si>
+    <t>2018-04-04</t>
+  </si>
+  <si>
+    <t>2018-04-05</t>
+  </si>
+  <si>
+    <t>2018-04-06</t>
+  </si>
+  <si>
+    <t>2018-04-07</t>
+  </si>
+  <si>
+    <t>2018-04-08</t>
+  </si>
+  <si>
+    <t>2018-04-09</t>
+  </si>
+  <si>
+    <t>2018-04-10</t>
+  </si>
+  <si>
+    <t>2018-04-11</t>
+  </si>
+  <si>
+    <t>2018-04-12</t>
+  </si>
+  <si>
+    <t>2018-04-13</t>
+  </si>
+  <si>
+    <t>2018-04-14</t>
+  </si>
+  <si>
+    <t>2018-04-15</t>
+  </si>
+  <si>
+    <t>2018-04-16</t>
+  </si>
+  <si>
+    <t>2018-04-17</t>
+  </si>
+  <si>
+    <t>2018-04-18</t>
+  </si>
+  <si>
+    <t>2018-04-19</t>
+  </si>
+  <si>
+    <t>2018-04-20</t>
+  </si>
+  <si>
+    <t>2018-04-21</t>
+  </si>
+  <si>
+    <t>2018-04-22</t>
+  </si>
+  <si>
+    <t>2018-04-23</t>
+  </si>
+  <si>
+    <t>2018-04-24</t>
+  </si>
+  <si>
+    <t>2018-04-25</t>
+  </si>
+  <si>
+    <t>2018-04-26</t>
+  </si>
+  <si>
+    <t>2018-04-27</t>
+  </si>
+  <si>
+    <t>2018-04-28</t>
+  </si>
+  <si>
+    <t>2018-04-29</t>
+  </si>
+  <si>
+    <t>2018-04-30</t>
+  </si>
+  <si>
+    <t>2018-05-01</t>
+  </si>
+  <si>
+    <t>2018-05-02</t>
+  </si>
+  <si>
+    <t>2018-05-03</t>
+  </si>
+  <si>
+    <t>2018-05-04</t>
+  </si>
+  <si>
+    <t>2018-05-05</t>
+  </si>
+  <si>
+    <t>2018-05-06</t>
+  </si>
+  <si>
+    <t>2018-05-07</t>
+  </si>
+  <si>
+    <t>2018-05-08</t>
+  </si>
+  <si>
+    <t>2018-05-09</t>
+  </si>
+  <si>
+    <t>2018-05-10</t>
+  </si>
+  <si>
+    <t>2018-05-11</t>
+  </si>
+  <si>
+    <t>2018-05-12</t>
+  </si>
+  <si>
+    <t>2018-05-13</t>
+  </si>
+  <si>
+    <t>2018-05-14</t>
+  </si>
+  <si>
+    <t>2018-05-15</t>
+  </si>
+  <si>
+    <t>2018-05-16</t>
+  </si>
+  <si>
+    <t>2018-05-17</t>
+  </si>
+  <si>
+    <t>2018-05-18</t>
+  </si>
+  <si>
+    <t>2018-05-19</t>
+  </si>
+  <si>
+    <t>2018-05-20</t>
+  </si>
+  <si>
+    <t>2018-05-21</t>
+  </si>
+  <si>
+    <t>2018-05-22</t>
+  </si>
+  <si>
+    <t>2018-05-23</t>
+  </si>
+  <si>
+    <t>2018-05-24</t>
+  </si>
+  <si>
+    <t>2018-05-25</t>
+  </si>
+  <si>
+    <t>2018-05-26</t>
+  </si>
+  <si>
+    <t>2018-05-27</t>
+  </si>
+  <si>
+    <t>2018-05-28</t>
+  </si>
+  <si>
+    <t>2018-05-29</t>
+  </si>
+  <si>
+    <t>2018-05-30</t>
+  </si>
+  <si>
+    <t>2018-05-31</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>91</t>
+  </si>
+  <si>
+    <t>92</t>
+  </si>
+  <si>
+    <t>93</t>
+  </si>
+  <si>
+    <t>94</t>
+  </si>
+  <si>
+    <t>95</t>
+  </si>
+  <si>
+    <t>96</t>
+  </si>
+  <si>
+    <t>97</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>102</t>
+  </si>
+  <si>
+    <t>103</t>
+  </si>
+  <si>
+    <t>104</t>
+  </si>
+  <si>
+    <t>105</t>
+  </si>
+  <si>
+    <t>106</t>
+  </si>
+  <si>
+    <t>107</t>
+  </si>
+  <si>
+    <t>108</t>
+  </si>
+  <si>
+    <t>109</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>112</t>
+  </si>
+  <si>
+    <t>113</t>
+  </si>
+  <si>
+    <t>114</t>
+  </si>
+  <si>
+    <t>115</t>
+  </si>
+  <si>
+    <t>116</t>
+  </si>
+  <si>
+    <t>117</t>
+  </si>
+  <si>
+    <t>118</t>
+  </si>
+  <si>
+    <t>119</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>121</t>
+  </si>
+  <si>
+    <t>122</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>125</t>
+  </si>
+  <si>
+    <t>126</t>
+  </si>
+  <si>
+    <t>127</t>
+  </si>
+  <si>
+    <t>128</t>
+  </si>
+  <si>
+    <t>129</t>
+  </si>
+  <si>
+    <t>130</t>
+  </si>
+  <si>
+    <t>131</t>
+  </si>
+  <si>
+    <t>132</t>
+  </si>
+  <si>
+    <t>133</t>
+  </si>
+  <si>
+    <t>134</t>
+  </si>
+  <si>
+    <t>135</t>
+  </si>
+  <si>
+    <t>136</t>
+  </si>
+  <si>
+    <t>137</t>
+  </si>
+  <si>
+    <t>138</t>
+  </si>
+  <si>
+    <t>139</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>141</t>
+  </si>
+  <si>
+    <t>142</t>
+  </si>
+  <si>
+    <t>143</t>
+  </si>
+  <si>
+    <t>144</t>
+  </si>
+  <si>
+    <t>145</t>
+  </si>
+  <si>
+    <t>146</t>
+  </si>
+  <si>
+    <t>147</t>
+  </si>
+  <si>
+    <t>148</t>
+  </si>
+  <si>
+    <t>149</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>2018-06-01</t>
+  </si>
+  <si>
+    <t>2018-06-02</t>
+  </si>
+  <si>
+    <t>2018-06-03</t>
+  </si>
+  <si>
+    <t>2018-06-04</t>
+  </si>
+  <si>
+    <t>2018-06-05</t>
+  </si>
+  <si>
+    <t>2018-06-06</t>
+  </si>
+  <si>
+    <t>2018-06-07</t>
+  </si>
+  <si>
+    <t>2018-06-08</t>
+  </si>
+  <si>
+    <t>2018-06-09</t>
+  </si>
+  <si>
+    <t>2018-06-10</t>
+  </si>
+  <si>
+    <t>2018-06-11</t>
+  </si>
+  <si>
+    <t>2018-06-12</t>
+  </si>
+  <si>
+    <t>2018-06-13</t>
+  </si>
+  <si>
+    <t>2018-06-14</t>
+  </si>
+  <si>
+    <t>2018-06-15</t>
+  </si>
+  <si>
+    <t>2018-06-16</t>
+  </si>
+  <si>
+    <t>2018-06-17</t>
+  </si>
+  <si>
+    <t>2018-06-18</t>
+  </si>
+  <si>
+    <t>2018-06-19</t>
+  </si>
+  <si>
+    <t>2018-06-20</t>
+  </si>
+  <si>
+    <t>2018-06-21</t>
+  </si>
+  <si>
+    <t>2018-06-22</t>
+  </si>
+  <si>
+    <t>2018-06-23</t>
+  </si>
+  <si>
+    <t>2018-06-24</t>
+  </si>
+  <si>
+    <t>2018-06-25</t>
+  </si>
+  <si>
+    <t>2018-06-26</t>
+  </si>
+  <si>
+    <t>2018-06-27</t>
+  </si>
+  <si>
+    <t>2018-06-28</t>
+  </si>
+  <si>
+    <t>2018-06-29</t>
+  </si>
+  <si>
+    <t>2018-06-30</t>
+  </si>
+  <si>
+    <t>2018-07-01</t>
+  </si>
+  <si>
+    <t>2018-07-02</t>
+  </si>
+  <si>
+    <t>2018-07-03</t>
+  </si>
+  <si>
+    <t>2018-07-04</t>
+  </si>
+  <si>
+    <t>2018-07-05</t>
+  </si>
+  <si>
+    <t>2018-07-06</t>
+  </si>
+  <si>
+    <t>2018-07-07</t>
+  </si>
+  <si>
+    <t>2018-07-08</t>
+  </si>
+  <si>
+    <t>2018-07-09</t>
+  </si>
+  <si>
+    <t>2018-07-10</t>
+  </si>
+  <si>
+    <t>2018-07-11</t>
+  </si>
+  <si>
+    <t>2018-07-12</t>
+  </si>
+  <si>
+    <t>2018-07-13</t>
+  </si>
+  <si>
+    <t>2018-07-14</t>
+  </si>
+  <si>
+    <t>2018-07-15</t>
+  </si>
+  <si>
+    <t>2018-07-16</t>
+  </si>
+  <si>
+    <t>2018-07-17</t>
+  </si>
+  <si>
+    <t>2018-07-18</t>
+  </si>
+  <si>
+    <t>2018-07-19</t>
+  </si>
+  <si>
+    <t>2018-07-20</t>
+  </si>
+  <si>
+    <t>2018-07-21</t>
+  </si>
+  <si>
+    <t>2018-07-22</t>
+  </si>
+  <si>
+    <t>2018-07-23</t>
+  </si>
+  <si>
+    <t>2018-07-24</t>
+  </si>
+  <si>
+    <t>2018-07-25</t>
+  </si>
+  <si>
+    <t>2018-07-26</t>
+  </si>
+  <si>
+    <t>2018-07-27</t>
+  </si>
+  <si>
+    <t>2018-07-28</t>
+  </si>
+  <si>
+    <t>2018-07-29</t>
+  </si>
+  <si>
+    <t>2018-07-30</t>
+  </si>
+  <si>
+    <t>2018-07-31</t>
+  </si>
+  <si>
+    <t>151</t>
+  </si>
+  <si>
+    <t>152</t>
+  </si>
+  <si>
+    <t>153</t>
+  </si>
+  <si>
+    <t>154</t>
+  </si>
+  <si>
+    <t>155</t>
+  </si>
+  <si>
+    <t>156</t>
+  </si>
+  <si>
+    <t>157</t>
+  </si>
+  <si>
+    <t>158</t>
+  </si>
+  <si>
+    <t>159</t>
+  </si>
+  <si>
+    <t>160</t>
+  </si>
+  <si>
+    <t>161</t>
+  </si>
+  <si>
+    <t>162</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -650,7 +1380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -658,6 +1388,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -667,6 +1398,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -937,8 +1671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C90"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="G81" sqref="G81"/>
+    <sheetView showRuler="0" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1943,4 +2677,1859 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C171"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A131" workbookViewId="0">
+      <selection activeCell="F157" sqref="F157"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" s="3" t="s">
+        <v>276</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A116" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A117" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A118" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A119" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A120" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A121" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A122" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A123" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A124" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A125" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A126" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A127" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="C127" s="3" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A128" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A129" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A130" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A131" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A132" s="3" t="s">
+        <v>380</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A133" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A134" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A135" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A136" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A137" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A138" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A139" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="C139" s="3" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A140" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="C140" s="3" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A141" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="C141" s="3" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A142" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="B142" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C142" s="3" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A143" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="C143" s="3" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A144" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="B144" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="C144" s="3" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A145" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="C145" s="3" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A146" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="B146" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A147" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="C147" s="3" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A148" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="B148" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="C148" s="3" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A149" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="C149" s="3" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A150" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="B150" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C150" s="3" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A151" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="C151" s="3" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A152" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="B152" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="C152" s="3" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A153" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C153" s="3" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A154" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="C154" s="3" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A155" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="C155" s="3" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A156" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="B156" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="C156" s="3" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A157" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="C157" s="3" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A158" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="B158" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="C158" s="3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A159" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="C159" s="3" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A160" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="B160" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="C160" s="3" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A161" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="C161" s="3" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A162" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="B162" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="C162" s="3" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A163" s="3" t="s">
+        <v>411</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="C163" s="3" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A164" s="3" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A165" s="3" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A166" s="3" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A167" s="3" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A168" s="3" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A169" s="3" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A170" s="3" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A171" s="3" t="s">
+        <v>419</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>